<commit_message>
Pushed back sprints on Product Backlog
</commit_message>
<xml_diff>
--- a/Deliverable_2_Documents/FiveGuys_Deliverable_2_Product_Backlog.xlsx
+++ b/Deliverable_2_Documents/FiveGuys_Deliverable_2_Product_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xinophilius\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xinophilius\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8C915FE-AB20-401B-976D-1D71271B7D7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49F1929-C86E-467C-9D69-1A0179E3C870}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="930" windowWidth="25695" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>As a potential new user, I would like a built in tutorial, so that I can learn the game without having to look up a guide.</t>
+  </si>
+  <si>
+    <t>2 and 3</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -209,6 +212,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +530,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -594,8 +598,8 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -618,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -641,7 +645,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -664,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -687,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -707,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -727,7 +731,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -747,7 +751,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -767,7 +771,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -787,7 +791,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -807,7 +811,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -827,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -847,7 +851,7 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -867,7 +871,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -887,7 +891,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -927,7 +931,7 @@
         <v>31</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -947,7 +951,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -967,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -987,7 +991,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -1007,7 +1011,7 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1027,7 +1031,7 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1047,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -1067,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1087,7 +1091,7 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <v>5</v>
@@ -1107,7 +1111,7 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>5</v>

</xml_diff>